<commit_message>
[gfx][gl_wrapper] Window class pt 1
</commit_message>
<xml_diff>
--- a/docs/doc.xlsx
+++ b/docs/doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\CPP\games\honey_engine\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C54D8E7-1B3D-499D-8915-70554F33A00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE9C4B6-D6BD-4648-94BD-F813D94542C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="83">
   <si>
     <t>How To Render CIRCLES (OpenGL/Vulkan/DirectX/Metal)</t>
   </si>
@@ -272,6 +272,9 @@
   </si>
   <si>
     <t>Make saving log on a disk</t>
+  </si>
+  <si>
+    <t>Point2d powinien mieć prefix gfx</t>
   </si>
 </sst>
 </file>
@@ -661,7 +664,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,10 +775,16 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
+      <c r="B8" s="8">
+        <v>2</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>79</v>
+      </c>
       <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="E8" s="7" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>

</xml_diff>